<commit_message>
Pivoting to Mapbox and GeoJSON of school districts.
</commit_message>
<xml_diff>
--- a/data/nc_lateral_entry_by_county.xlsx
+++ b/data/nc_lateral_entry_by_county.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="35040" yWindow="3960" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="36240" yWindow="0" windowWidth="38900" windowHeight="26260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -383,12 +383,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -403,9 +409,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -739,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B115"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A115" sqref="A115:B115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -758,34 +768,34 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="3">
         <v>9.3655586242675795E-2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="3">
         <v>6.5040647983550998E-2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="3">
         <v>0.24336282908916498</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="3">
         <v>8.0168776214122814E-2</v>
       </c>
     </row>
@@ -806,106 +816,106 @@
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="3">
         <v>4.0229886770248406E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="3">
         <v>0.11834319680929201</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="3">
         <v>0.25698325037956199</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="3">
         <v>0.26708075404167197</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="3">
         <v>0.136250004172325</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="3">
         <v>7.4481077492237105E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="3">
         <v>0.15563724935054801</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="3">
         <v>0.104423865675926</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="3">
         <v>0.106257379055023</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="3">
         <v>0.152671754360199</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="3">
         <v>0.10107197612524001</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="3">
         <v>0.13131313025951399</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="3">
         <v>0.11649580299854299</v>
       </c>
     </row>
@@ -918,42 +928,42 @@
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" t="s">
+      <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="3">
         <v>0.170858830213547</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" t="s">
+      <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="3">
         <v>0.14900662004947698</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" t="s">
+      <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="3">
         <v>8.0321282148361206E-2</v>
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" t="s">
+      <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="3">
         <v>9.2783503234386402E-2</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" t="s">
+      <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="3">
         <v>0.16977778077125499</v>
       </c>
     </row>
@@ -966,74 +976,74 @@
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" t="s">
+      <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="3">
         <v>0.192941173911095</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" t="s">
+      <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="3">
         <v>0.13865546882152599</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" t="s">
+      <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30" s="3">
         <v>0.218697354197502</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" t="s">
+      <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" s="3">
         <v>8.2677163183689104E-2</v>
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" t="s">
+      <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="3">
         <v>0.115089513361454</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" t="s">
+      <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" s="3">
         <v>0.16338258981704701</v>
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" t="s">
+      <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="3">
         <v>0.11486486345529601</v>
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" t="s">
+      <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35" s="3">
         <v>0.185126587748528</v>
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" t="s">
+      <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36" s="3">
         <v>0.184729069471359</v>
       </c>
     </row>
@@ -1046,10 +1056,10 @@
       </c>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38" t="s">
+      <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="3">
         <v>0.19900497794151298</v>
       </c>
     </row>
@@ -1070,98 +1080,98 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" t="s">
+      <c r="A41" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="3">
         <v>0.221441119909287</v>
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" t="s">
+      <c r="A42" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="1">
+      <c r="B42" s="3">
         <v>0.15546433627605399</v>
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" t="s">
+      <c r="A43" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B43" s="3">
         <v>0.16296295821666701</v>
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" t="s">
+      <c r="A44" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B44" s="3">
         <v>5.4945055395364796E-2</v>
       </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" t="s">
+      <c r="A45" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B45" s="3">
         <v>0.141975313425064</v>
       </c>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" t="s">
+      <c r="A46" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="1">
+      <c r="B46" s="3">
         <v>0.10047847032547001</v>
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" t="s">
+      <c r="A47" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B47" s="3">
         <v>0.194461420178413</v>
       </c>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" t="s">
+      <c r="A48" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48" s="3">
         <v>0.318385660648346</v>
       </c>
     </row>
     <row r="49" spans="1:2">
-      <c r="A49" t="s">
+      <c r="A49" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="3">
         <v>0.19137254357338002</v>
       </c>
     </row>
     <row r="50" spans="1:2">
-      <c r="A50" t="s">
+      <c r="A50" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B50" s="1">
+      <c r="B50" s="3">
         <v>9.7378276288509411E-2</v>
       </c>
     </row>
     <row r="51" spans="1:2">
-      <c r="A51" t="s">
+      <c r="A51" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B51" s="5">
         <v>0.102508179843426</v>
       </c>
     </row>
     <row r="52" spans="1:2">
-      <c r="A52" t="s">
+      <c r="A52" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B52" s="1">
+      <c r="B52" s="3">
         <v>0.308056861162186</v>
       </c>
     </row>
@@ -1174,18 +1184,18 @@
       </c>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" t="s">
+      <c r="A54" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B54" s="1">
+      <c r="B54" s="3">
         <v>0.23550087213516199</v>
       </c>
     </row>
     <row r="55" spans="1:2">
-      <c r="A55" t="s">
+      <c r="A55" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B55" s="1">
+      <c r="B55" s="5">
         <v>0.10000000149011599</v>
       </c>
     </row>
@@ -1198,26 +1208,26 @@
       </c>
     </row>
     <row r="57" spans="1:2">
-      <c r="A57" t="s">
+      <c r="A57" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B57" s="3">
         <v>0.11023622006177901</v>
       </c>
     </row>
     <row r="58" spans="1:2">
-      <c r="A58" t="s">
+      <c r="A58" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B58" s="3">
         <v>0.164329528808594</v>
       </c>
     </row>
     <row r="59" spans="1:2">
-      <c r="A59" t="s">
+      <c r="A59" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B59" s="3">
         <v>0.18888889253139499</v>
       </c>
     </row>
@@ -1230,18 +1240,18 @@
       </c>
     </row>
     <row r="61" spans="1:2">
-      <c r="A61" t="s">
+      <c r="A61" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B61" s="1">
+      <c r="B61" s="3">
         <v>0.11885895580053299</v>
       </c>
     </row>
     <row r="62" spans="1:2">
-      <c r="A62" t="s">
+      <c r="A62" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B62" s="1">
+      <c r="B62" s="3">
         <v>0.174872666597366</v>
       </c>
     </row>
@@ -1254,66 +1264,66 @@
       </c>
     </row>
     <row r="64" spans="1:2">
-      <c r="A64" t="s">
+      <c r="A64" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B64" s="1">
+      <c r="B64" s="3">
         <v>0.13121019303798701</v>
       </c>
     </row>
     <row r="65" spans="1:2">
-      <c r="A65" t="s">
+      <c r="A65" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B65" s="1">
+      <c r="B65" s="3">
         <v>0.10248447209596601</v>
       </c>
     </row>
     <row r="66" spans="1:2">
-      <c r="A66" t="s">
+      <c r="A66" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B66" s="1">
+      <c r="B66" s="3">
         <v>0.12565444409847301</v>
       </c>
     </row>
     <row r="67" spans="1:2">
-      <c r="A67" t="s">
+      <c r="A67" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B67" s="1">
+      <c r="B67" s="3">
         <v>0.146718144416809</v>
       </c>
     </row>
     <row r="68" spans="1:2">
-      <c r="A68" t="s">
+      <c r="A68" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B68" s="1">
+      <c r="B68" s="3">
         <v>0.12814645469188701</v>
       </c>
     </row>
     <row r="69" spans="1:2">
-      <c r="A69" t="s">
+      <c r="A69" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B69" s="1">
+      <c r="B69" s="3">
         <v>3.9735101163387299E-2</v>
       </c>
     </row>
     <row r="70" spans="1:2">
-      <c r="A70" t="s">
+      <c r="A70" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B70" s="1">
+      <c r="B70" s="3">
         <v>0.20136518776416801</v>
       </c>
     </row>
     <row r="71" spans="1:2">
-      <c r="A71" t="s">
+      <c r="A71" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B71" s="3">
         <v>0.17460317909717599</v>
       </c>
     </row>
@@ -1342,10 +1352,10 @@
       </c>
     </row>
     <row r="75" spans="1:2">
-      <c r="A75" t="s">
+      <c r="A75" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B75" s="1">
+      <c r="B75" s="3">
         <v>8.5380837321281391E-2</v>
       </c>
     </row>
@@ -1358,90 +1368,90 @@
       </c>
     </row>
     <row r="77" spans="1:2">
-      <c r="A77" t="s">
+      <c r="A77" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B77" s="1">
+      <c r="B77" s="3">
         <v>0.227272734045982</v>
       </c>
     </row>
     <row r="78" spans="1:2">
-      <c r="A78" t="s">
+      <c r="A78" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B78" s="1">
+      <c r="B78" s="3">
         <v>8.9430890977382702E-2</v>
       </c>
     </row>
     <row r="79" spans="1:2">
-      <c r="A79" t="s">
+      <c r="A79" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B79" s="1">
+      <c r="B79" s="3">
         <v>9.5840871334075886E-2</v>
       </c>
     </row>
     <row r="80" spans="1:2">
-      <c r="A80" t="s">
+      <c r="A80" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B80" s="1">
+      <c r="B80" s="3">
         <v>0.14285714924335499</v>
       </c>
     </row>
     <row r="81" spans="1:2">
-      <c r="A81" t="s">
+      <c r="A81" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B81" s="1">
+      <c r="B81" s="3">
         <v>9.107468277215959E-2</v>
       </c>
     </row>
     <row r="82" spans="1:2">
-      <c r="A82" t="s">
+      <c r="A82" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B82" s="1">
+      <c r="B82" s="3">
         <v>0.17741934955120101</v>
       </c>
     </row>
     <row r="83" spans="1:2">
-      <c r="A83" t="s">
+      <c r="A83" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B83" s="1">
+      <c r="B83" s="3">
         <v>0.18688525259494798</v>
       </c>
     </row>
     <row r="84" spans="1:2">
-      <c r="A84" t="s">
+      <c r="A84" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B84" s="1">
+      <c r="B84" s="3">
         <v>0.14092308282852201</v>
       </c>
     </row>
     <row r="85" spans="1:2">
-      <c r="A85" t="s">
+      <c r="A85" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B85" s="1">
+      <c r="B85" s="3">
         <v>9.6446700394153595E-2</v>
       </c>
     </row>
     <row r="86" spans="1:2">
-      <c r="A86" t="s">
+      <c r="A86" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B86" s="1">
+      <c r="B86" s="3">
         <v>0.18165938556194297</v>
       </c>
     </row>
     <row r="87" spans="1:2">
-      <c r="A87" t="s">
+      <c r="A87" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B87" s="1">
+      <c r="B87" s="3">
         <v>0.258382648229599</v>
       </c>
     </row>
@@ -1454,18 +1464,18 @@
       </c>
     </row>
     <row r="89" spans="1:2">
-      <c r="A89" t="s">
+      <c r="A89" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B89" s="1">
+      <c r="B89" s="3">
         <v>0.31585931777954102</v>
       </c>
     </row>
     <row r="90" spans="1:2">
-      <c r="A90" t="s">
+      <c r="A90" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B90" s="1">
+      <c r="B90" s="3">
         <v>0.15041127800941501</v>
       </c>
     </row>
@@ -1478,58 +1488,58 @@
       </c>
     </row>
     <row r="92" spans="1:2">
-      <c r="A92" t="s">
+      <c r="A92" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B92" s="1">
+      <c r="B92" s="3">
         <v>0.13743218779563901</v>
       </c>
     </row>
     <row r="93" spans="1:2">
-      <c r="A93" t="s">
+      <c r="A93" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B93" s="1">
+      <c r="B93" s="3">
         <v>0.25043782591819796</v>
       </c>
     </row>
     <row r="94" spans="1:2">
-      <c r="A94" t="s">
+      <c r="A94" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B94" s="1">
+      <c r="B94" s="3">
         <v>0.29748284816741899</v>
       </c>
     </row>
     <row r="95" spans="1:2">
-      <c r="A95" t="s">
+      <c r="A95" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B95" s="1">
+      <c r="B95" s="3">
         <v>0.18466353416442899</v>
       </c>
     </row>
     <row r="96" spans="1:2">
-      <c r="A96" t="s">
+      <c r="A96" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B96" s="1">
+      <c r="B96" s="3">
         <v>0.14675052464008298</v>
       </c>
     </row>
     <row r="97" spans="1:2">
-      <c r="A97" t="s">
+      <c r="A97" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B97" s="1">
+      <c r="B97" s="3">
         <v>0.123655915260315</v>
       </c>
     </row>
     <row r="98" spans="1:2">
-      <c r="A98" t="s">
+      <c r="A98" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B98" s="1">
+      <c r="B98" s="3">
         <v>0.129251703619957</v>
       </c>
     </row>
@@ -1542,74 +1552,74 @@
       </c>
     </row>
     <row r="100" spans="1:2">
-      <c r="A100" t="s">
+      <c r="A100" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B100" s="1">
+      <c r="B100" s="3">
         <v>9.8939932882785797E-2</v>
       </c>
     </row>
     <row r="101" spans="1:2">
-      <c r="A101" t="s">
+      <c r="A101" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B101" s="1">
+      <c r="B101" s="3">
         <v>0.150943398475647</v>
       </c>
     </row>
     <row r="102" spans="1:2">
-      <c r="A102" t="s">
+      <c r="A102" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B102" s="1">
+      <c r="B102" s="3">
         <v>0.13926941156387301</v>
       </c>
     </row>
     <row r="103" spans="1:2">
-      <c r="A103" t="s">
+      <c r="A103" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B103" s="1">
+      <c r="B103" s="3">
         <v>0.27777779102325401</v>
       </c>
     </row>
     <row r="104" spans="1:2">
-      <c r="A104" t="s">
+      <c r="A104" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B104" s="1">
+      <c r="B104" s="3">
         <v>0.103654943406582</v>
       </c>
     </row>
     <row r="105" spans="1:2">
-      <c r="A105" t="s">
+      <c r="A105" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B105" s="1">
+      <c r="B105" s="3">
         <v>0.22941176593303703</v>
       </c>
     </row>
     <row r="106" spans="1:2">
-      <c r="A106" t="s">
+      <c r="A106" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B106" s="1">
+      <c r="B106" s="3">
         <v>0.19444444775581399</v>
       </c>
     </row>
     <row r="107" spans="1:2">
-      <c r="A107" t="s">
+      <c r="A107" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B107" s="1">
+      <c r="B107" s="3">
         <v>5.8171745389699901E-2</v>
       </c>
     </row>
     <row r="108" spans="1:2">
-      <c r="A108" t="s">
+      <c r="A108" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B108" s="1">
+      <c r="B108" s="3">
         <v>0.26294821500778198</v>
       </c>
     </row>
@@ -1630,42 +1640,42 @@
       </c>
     </row>
     <row r="111" spans="1:2">
-      <c r="A111" t="s">
+      <c r="A111" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B111" s="1">
+      <c r="B111" s="3">
         <v>8.3333335816860199E-2</v>
       </c>
     </row>
     <row r="112" spans="1:2">
-      <c r="A112" t="s">
+      <c r="A112" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B112" s="1">
+      <c r="B112" s="3">
         <v>0.20478723943233501</v>
       </c>
     </row>
     <row r="113" spans="1:2">
-      <c r="A113" t="s">
+      <c r="A113" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B113" s="1">
+      <c r="B113" s="3">
         <v>0.17482334375381503</v>
       </c>
     </row>
     <row r="114" spans="1:2">
-      <c r="A114" t="s">
+      <c r="A114" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B114" s="1">
+      <c r="B114" s="3">
         <v>0.17142857611179402</v>
       </c>
     </row>
     <row r="115" spans="1:2">
-      <c r="A115" t="s">
+      <c r="A115" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B115" s="1">
+      <c r="B115" s="3">
         <v>0.102272726595402</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated message for not applicable school districts.
</commit_message>
<xml_diff>
--- a/data/nc_lateral_entry_by_county.xlsx
+++ b/data/nc_lateral_entry_by_county.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="36240" yWindow="0" windowWidth="38900" windowHeight="26260" tabRatio="500"/>
+    <workbookView xWindow="2160" yWindow="700" windowWidth="25360" windowHeight="14860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -379,11 +379,10 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="128"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -393,6 +392,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -409,13 +414,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -749,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A115" sqref="A115:B115"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="A114" sqref="A114:B114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -760,922 +766,922 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B1" s="2">
         <v>0.152887140019379</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>9.3655586242675795E-2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>6.5040647983550998E-2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>0.24336282908916498</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>8.0168776214122814E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="2">
         <v>0.16292135417461398</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="2">
         <v>9.2024542391300201E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>4.0229886770248406E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>0.11834319680929201</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>0.25698325037956199</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>0.26708075404167197</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>0.136250004172325</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>7.4481077492237105E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>0.15563724935054801</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>0.104423865675926</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <v>0.106257379055023</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>0.152671754360199</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <v>0.10107197612524001</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="2">
         <v>0.13131313025951399</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="2">
         <v>0.11649580299854299</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="2">
         <v>8.6580090224742903E-2</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <v>0.170858830213547</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="2">
         <v>0.14900662004947698</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="2">
         <v>8.0321282148361206E-2</v>
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="2">
         <v>9.2783503234386402E-2</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="2">
         <v>0.16977778077125499</v>
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" t="s">
+      <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="2">
         <v>0.22330096364021301</v>
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="2">
         <v>0.192941173911095</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="2">
         <v>0.13865546882152599</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="2">
         <v>0.218697354197502</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="2">
         <v>8.2677163183689104E-2</v>
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="2">
         <v>0.115089513361454</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="2">
         <v>0.16338258981704701</v>
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="2">
         <v>0.11486486345529601</v>
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="2">
         <v>0.185126587748528</v>
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="2">
         <v>0.184729069471359</v>
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" t="s">
+      <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="2">
         <v>7.1895428001880604E-2</v>
       </c>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="2">
         <v>0.19900497794151298</v>
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" t="s">
+      <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="2">
         <v>0.19487179815769198</v>
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" t="s">
+      <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="2">
         <v>0.11340206116437899</v>
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B41" s="2">
         <v>0.221441119909287</v>
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B42" s="2">
         <v>0.15546433627605399</v>
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43" s="2">
         <v>0.16296295821666701</v>
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44" s="2">
         <v>5.4945055395364796E-2</v>
       </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B45" s="2">
         <v>0.141975313425064</v>
       </c>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B46" s="2">
         <v>0.10047847032547001</v>
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B47" s="2">
         <v>0.194461420178413</v>
       </c>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B48" s="2">
         <v>0.318385660648346</v>
       </c>
     </row>
     <row r="49" spans="1:2">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B49" s="2">
         <v>0.19137254357338002</v>
       </c>
     </row>
     <row r="50" spans="1:2">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B50" s="3">
+      <c r="B50" s="2">
         <v>9.7378276288509411E-2</v>
       </c>
     </row>
     <row r="51" spans="1:2">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="5">
+      <c r="B51" s="4">
         <v>0.102508179843426</v>
       </c>
     </row>
     <row r="52" spans="1:2">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B52" s="3">
+      <c r="B52" s="2">
         <v>0.308056861162186</v>
       </c>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53" t="s">
+      <c r="A53" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B53" s="1">
+      <c r="B53" s="2">
         <v>0.104026846587658</v>
       </c>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="2" t="s">
+      <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B54" s="3">
+      <c r="B54" s="2">
         <v>0.23550087213516199</v>
       </c>
     </row>
     <row r="55" spans="1:2">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B55" s="5">
+      <c r="B55" s="4">
         <v>0.10000000149011599</v>
       </c>
     </row>
     <row r="56" spans="1:2">
-      <c r="A56" t="s">
+      <c r="A56" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B56" s="1">
+      <c r="B56" s="2">
         <v>0.129900082945824</v>
       </c>
     </row>
     <row r="57" spans="1:2">
-      <c r="A57" s="2" t="s">
+      <c r="A57" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B57" s="3">
+      <c r="B57" s="2">
         <v>0.11023622006177901</v>
       </c>
     </row>
     <row r="58" spans="1:2">
-      <c r="A58" s="2" t="s">
+      <c r="A58" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B58" s="3">
+      <c r="B58" s="2">
         <v>0.164329528808594</v>
       </c>
     </row>
     <row r="59" spans="1:2">
-      <c r="A59" s="2" t="s">
+      <c r="A59" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B59" s="3">
+      <c r="B59" s="2">
         <v>0.18888889253139499</v>
       </c>
     </row>
     <row r="60" spans="1:2">
-      <c r="A60" t="s">
+      <c r="A60" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B60" s="2">
         <v>0.102631576359272</v>
       </c>
     </row>
     <row r="61" spans="1:2">
-      <c r="A61" s="2" t="s">
+      <c r="A61" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B61" s="3">
+      <c r="B61" s="2">
         <v>0.11885895580053299</v>
       </c>
     </row>
     <row r="62" spans="1:2">
-      <c r="A62" s="2" t="s">
+      <c r="A62" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B62" s="3">
+      <c r="B62" s="2">
         <v>0.174872666597366</v>
       </c>
     </row>
     <row r="63" spans="1:2">
-      <c r="A63" t="s">
+      <c r="A63" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B63" s="1">
+      <c r="B63" s="2">
         <v>0.180995479226112</v>
       </c>
     </row>
     <row r="64" spans="1:2">
-      <c r="A64" s="2" t="s">
+      <c r="A64" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B64" s="3">
+      <c r="B64" s="2">
         <v>0.13121019303798701</v>
       </c>
     </row>
     <row r="65" spans="1:2">
-      <c r="A65" s="2" t="s">
+      <c r="A65" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B65" s="3">
+      <c r="B65" s="2">
         <v>0.10248447209596601</v>
       </c>
     </row>
     <row r="66" spans="1:2">
-      <c r="A66" s="2" t="s">
+      <c r="A66" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B66" s="3">
+      <c r="B66" s="2">
         <v>0.12565444409847301</v>
       </c>
     </row>
     <row r="67" spans="1:2">
-      <c r="A67" s="2" t="s">
+      <c r="A67" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B67" s="3">
+      <c r="B67" s="2">
         <v>0.146718144416809</v>
       </c>
     </row>
     <row r="68" spans="1:2">
-      <c r="A68" s="2" t="s">
+      <c r="A68" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B68" s="3">
+      <c r="B68" s="2">
         <v>0.12814645469188701</v>
       </c>
     </row>
     <row r="69" spans="1:2">
-      <c r="A69" s="2" t="s">
+      <c r="A69" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B69" s="3">
+      <c r="B69" s="2">
         <v>3.9735101163387299E-2</v>
       </c>
     </row>
     <row r="70" spans="1:2">
-      <c r="A70" s="2" t="s">
+      <c r="A70" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B70" s="3">
+      <c r="B70" s="2">
         <v>0.20136518776416801</v>
       </c>
     </row>
     <row r="71" spans="1:2">
-      <c r="A71" s="2" t="s">
+      <c r="A71" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B71" s="3">
+      <c r="B71" s="2">
         <v>0.17460317909717599</v>
       </c>
     </row>
     <row r="72" spans="1:2">
-      <c r="A72" t="s">
+      <c r="A72" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B72" s="1">
+      <c r="B72" s="2">
         <v>0.119891010224819</v>
       </c>
     </row>
     <row r="73" spans="1:2">
-      <c r="A73" t="s">
+      <c r="A73" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B73" s="2">
         <v>0.104000002145767</v>
       </c>
     </row>
     <row r="74" spans="1:2">
-      <c r="A74" t="s">
+      <c r="A74" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B74" s="1">
+      <c r="B74" s="2">
         <v>0.24893617630004899</v>
       </c>
     </row>
     <row r="75" spans="1:2">
-      <c r="A75" s="2" t="s">
+      <c r="A75" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B75" s="3">
+      <c r="B75" s="2">
         <v>8.5380837321281391E-2</v>
       </c>
     </row>
     <row r="76" spans="1:2">
-      <c r="A76" t="s">
+      <c r="A76" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B76" s="1">
+      <c r="B76" s="2">
         <v>0.15887850522995001</v>
       </c>
     </row>
     <row r="77" spans="1:2">
-      <c r="A77" s="2" t="s">
+      <c r="A77" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B77" s="3">
+      <c r="B77" s="2">
         <v>0.227272734045982</v>
       </c>
     </row>
     <row r="78" spans="1:2">
-      <c r="A78" s="2" t="s">
+      <c r="A78" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B78" s="3">
+      <c r="B78" s="2">
         <v>8.9430890977382702E-2</v>
       </c>
     </row>
     <row r="79" spans="1:2">
-      <c r="A79" s="2" t="s">
+      <c r="A79" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B79" s="3">
+      <c r="B79" s="2">
         <v>9.5840871334075886E-2</v>
       </c>
     </row>
     <row r="80" spans="1:2">
-      <c r="A80" s="2" t="s">
+      <c r="A80" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B80" s="3">
+      <c r="B80" s="2">
         <v>0.14285714924335499</v>
       </c>
     </row>
     <row r="81" spans="1:2">
-      <c r="A81" s="2" t="s">
+      <c r="A81" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B81" s="3">
+      <c r="B81" s="2">
         <v>9.107468277215959E-2</v>
       </c>
     </row>
     <row r="82" spans="1:2">
-      <c r="A82" s="2" t="s">
+      <c r="A82" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B82" s="3">
+      <c r="B82" s="2">
         <v>0.17741934955120101</v>
       </c>
     </row>
     <row r="83" spans="1:2">
-      <c r="A83" s="2" t="s">
+      <c r="A83" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B83" s="3">
+      <c r="B83" s="2">
         <v>0.18688525259494798</v>
       </c>
     </row>
     <row r="84" spans="1:2">
-      <c r="A84" s="2" t="s">
+      <c r="A84" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B84" s="3">
+      <c r="B84" s="2">
         <v>0.14092308282852201</v>
       </c>
     </row>
     <row r="85" spans="1:2">
-      <c r="A85" s="2" t="s">
+      <c r="A85" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B85" s="3">
+      <c r="B85" s="2">
         <v>9.6446700394153595E-2</v>
       </c>
     </row>
     <row r="86" spans="1:2">
-      <c r="A86" s="2" t="s">
+      <c r="A86" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B86" s="3">
+      <c r="B86" s="2">
         <v>0.18165938556194297</v>
       </c>
     </row>
     <row r="87" spans="1:2">
-      <c r="A87" s="2" t="s">
+      <c r="A87" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B87" s="3">
+      <c r="B87" s="2">
         <v>0.258382648229599</v>
       </c>
     </row>
     <row r="88" spans="1:2">
-      <c r="A88" t="s">
+      <c r="A88" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B88" s="1">
+      <c r="B88" s="2">
         <v>0.15463916957378399</v>
       </c>
     </row>
     <row r="89" spans="1:2">
-      <c r="A89" s="2" t="s">
+      <c r="A89" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B89" s="3">
+      <c r="B89" s="2">
         <v>0.31585931777954102</v>
       </c>
     </row>
     <row r="90" spans="1:2">
-      <c r="A90" s="2" t="s">
+      <c r="A90" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B90" s="3">
+      <c r="B90" s="2">
         <v>0.15041127800941501</v>
       </c>
     </row>
     <row r="91" spans="1:2">
-      <c r="A91" t="s">
+      <c r="A91" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B91" s="1">
+      <c r="B91" s="2">
         <v>0.13803680241107899</v>
       </c>
     </row>
     <row r="92" spans="1:2">
-      <c r="A92" s="2" t="s">
+      <c r="A92" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B92" s="3">
+      <c r="B92" s="2">
         <v>0.13743218779563901</v>
       </c>
     </row>
     <row r="93" spans="1:2">
-      <c r="A93" s="2" t="s">
+      <c r="A93" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B93" s="3">
+      <c r="B93" s="2">
         <v>0.25043782591819796</v>
       </c>
     </row>
     <row r="94" spans="1:2">
-      <c r="A94" s="2" t="s">
+      <c r="A94" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B94" s="3">
+      <c r="B94" s="2">
         <v>0.29748284816741899</v>
       </c>
     </row>
     <row r="95" spans="1:2">
-      <c r="A95" s="2" t="s">
+      <c r="A95" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B95" s="3">
+      <c r="B95" s="2">
         <v>0.18466353416442899</v>
       </c>
     </row>
     <row r="96" spans="1:2">
-      <c r="A96" s="2" t="s">
+      <c r="A96" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B96" s="3">
+      <c r="B96" s="2">
         <v>0.14675052464008298</v>
       </c>
     </row>
     <row r="97" spans="1:2">
-      <c r="A97" s="2" t="s">
+      <c r="A97" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B97" s="3">
+      <c r="B97" s="2">
         <v>0.123655915260315</v>
       </c>
     </row>
     <row r="98" spans="1:2">
-      <c r="A98" s="2" t="s">
+      <c r="A98" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B98" s="3">
+      <c r="B98" s="2">
         <v>0.129251703619957</v>
       </c>
     </row>
     <row r="99" spans="1:2">
-      <c r="A99" t="s">
+      <c r="A99" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B99" s="1">
+      <c r="B99" s="2">
         <v>0.14545454084873199</v>
       </c>
     </row>
     <row r="100" spans="1:2">
-      <c r="A100" s="2" t="s">
+      <c r="A100" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B100" s="3">
+      <c r="B100" s="2">
         <v>9.8939932882785797E-2</v>
       </c>
     </row>
     <row r="101" spans="1:2">
-      <c r="A101" s="2" t="s">
+      <c r="A101" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B101" s="3">
+      <c r="B101" s="2">
         <v>0.150943398475647</v>
       </c>
     </row>
     <row r="102" spans="1:2">
-      <c r="A102" s="2" t="s">
+      <c r="A102" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B102" s="3">
+      <c r="B102" s="2">
         <v>0.13926941156387301</v>
       </c>
     </row>
     <row r="103" spans="1:2">
-      <c r="A103" s="2" t="s">
+      <c r="A103" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B103" s="3">
+      <c r="B103" s="2">
         <v>0.27777779102325401</v>
       </c>
     </row>
     <row r="104" spans="1:2">
-      <c r="A104" s="2" t="s">
+      <c r="A104" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B104" s="3">
+      <c r="B104" s="2">
         <v>0.103654943406582</v>
       </c>
     </row>
     <row r="105" spans="1:2">
-      <c r="A105" s="2" t="s">
+      <c r="A105" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B105" s="3">
+      <c r="B105" s="2">
         <v>0.22941176593303703</v>
       </c>
     </row>
     <row r="106" spans="1:2">
-      <c r="A106" s="2" t="s">
+      <c r="A106" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B106" s="3">
+      <c r="B106" s="2">
         <v>0.19444444775581399</v>
       </c>
     </row>
     <row r="107" spans="1:2">
-      <c r="A107" s="2" t="s">
+      <c r="A107" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B107" s="3">
+      <c r="B107" s="2">
         <v>5.8171745389699901E-2</v>
       </c>
     </row>
     <row r="108" spans="1:2">
-      <c r="A108" s="2" t="s">
+      <c r="A108" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B108" s="3">
+      <c r="B108" s="2">
         <v>0.26294821500778198</v>
       </c>
     </row>
     <row r="109" spans="1:2">
-      <c r="A109" t="s">
+      <c r="A109" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B109" s="1">
+      <c r="B109" s="2">
         <v>0.29113924503326399</v>
       </c>
     </row>
     <row r="110" spans="1:2">
-      <c r="A110" t="s">
+      <c r="A110" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B110" s="1">
+      <c r="B110" s="2">
         <v>0.19879518449306499</v>
       </c>
     </row>
     <row r="111" spans="1:2">
-      <c r="A111" s="2" t="s">
+      <c r="A111" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B111" s="3">
+      <c r="B111" s="2">
         <v>8.3333335816860199E-2</v>
       </c>
     </row>
     <row r="112" spans="1:2">
-      <c r="A112" s="2" t="s">
+      <c r="A112" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B112" s="3">
+      <c r="B112" s="2">
         <v>0.20478723943233501</v>
       </c>
     </row>
     <row r="113" spans="1:2">
-      <c r="A113" s="2" t="s">
+      <c r="A113" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B113" s="3">
+      <c r="B113" s="2">
         <v>0.17482334375381503</v>
       </c>
     </row>
     <row r="114" spans="1:2">
-      <c r="A114" s="2" t="s">
+      <c r="A114" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B114" s="3">
+      <c r="B114" s="2">
         <v>0.17142857611179402</v>
       </c>
     </row>
     <row r="115" spans="1:2">
-      <c r="A115" s="2" t="s">
+      <c r="A115" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B115" s="3">
+      <c r="B115" s="6">
         <v>0.102272726595402</v>
       </c>
     </row>

</xml_diff>